<commit_message>
- Remove complex tab from import spreadsheets - Remove scheduler subprocess calls - scheduler needs to be run in startup code, not launched later
</commit_message>
<xml_diff>
--- a/static/import/faculty_enrollment_template.xlsx
+++ b/static/import/faculty_enrollment_template.xlsx
@@ -1,14 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ray\Desktop\git_projects\ope\smc\static\import\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="19155" windowHeight="8505"/>
   </bookViews>
   <sheets>
-    <sheet name="SIMPLE SHEET" sheetId="1" r:id="rId1"/>
-    <sheet name="COMPLEX SHEET" sheetId="2" r:id="rId2"/>
+    <sheet name="FACULTY USERS" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="Time">#REF!</definedName>
@@ -18,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -35,25 +39,10 @@
     <t>Program</t>
   </si>
   <si>
-    <t>Credits</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Work Days</t>
-  </si>
-  <si>
     <t>Pulsipher, Ray</t>
   </si>
   <si>
-    <t>M-F</t>
-  </si>
-  <si>
     <t>CSE</t>
-  </si>
-  <si>
-    <t>Open Enrollment</t>
   </si>
   <si>
     <t>Peet, Gail</t>
@@ -141,6 +130,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -188,7 +180,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -223,7 +215,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -435,7 +427,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,7 +440,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -465,36 +457,36 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
         <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -513,173 +505,19 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2 H6">
-      <formula1>Time</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3">
-        <v>5</v>
-      </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>